<commit_message>
Updated data model for idrepo changes
</commit_message>
<xml_diff>
--- a/scripts/database/data_model/mosip_idrepo_dd.xlsx
+++ b/scripts/database/data_model/mosip_idrepo_dd.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work_Backup\NasirKhan\MindTree\Digital\Projects\MOSIP\Data Model\DataDictionary\Latest\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\mosip\scripts\database\data_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{CF557BC7-814B-452B-98A3-C856CAB5E5F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{D9AA5484-A669-448A-9A7D-82BFAEDDD985}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data Dictionary" sheetId="5" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1328" uniqueCount="124">
   <si>
     <t>cr_by</t>
   </si>
@@ -396,6 +396,9 @@
   </si>
   <si>
     <t>Salt: Random generated number used as salt to hash the uin field.</t>
+  </si>
+  <si>
+    <t>uk_uin_uin_hash</t>
   </si>
 </sst>
 </file>
@@ -804,9 +807,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC79934D-055A-430D-A368-EF7E2FBF9133}">
   <dimension ref="B1:J107"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -954,8 +955,12 @@
       <c r="H6" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
+      <c r="I6" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.2">
       <c r="B7" s="7" t="s">
@@ -3450,7 +3455,7 @@
   <dimension ref="B2:L100"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:L99"/>
+      <selection activeCell="J5" sqref="J5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3599,8 +3604,12 @@
       <c r="I5" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
+      <c r="J5" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>39</v>
+      </c>
       <c r="L5" s="2" t="s">
         <v>42</v>
       </c>
@@ -6552,7 +6561,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{97C824AA-3ED3-4FE1-A2F9-BAA02595C989}">
   <dimension ref="B2:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:L10"/>
     </sheetView>
   </sheetViews>

</xml_diff>